<commit_message>
recorte de imagenes para choco
</commit_message>
<xml_diff>
--- a/web_scraping_main/excel_a_json/prodcutos_reposteria_sin_imagen.xlsx
+++ b/web_scraping_main/excel_a_json/prodcutos_reposteria_sin_imagen.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FAA0315-3770-4980-9E64-C5C7BE43E718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
     <sheet name="prodcutos_reposteria" sheetId="3" r:id="rId1"/>
@@ -23,11 +22,11 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="Consulta - 2024-06-11 07-08-40" description="Conexión a la consulta '2024-06-11 07-08-40' en el libro." type="5" refreshedVersion="8" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" keepAlive="1" name="Consulta - 2024-06-11 07-08-40" description="Conexión a la consulta '2024-06-11 07-08-40' en el libro." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;2024-06-11 07-08-40&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [2024-06-11 07-08-40]"/>
   </connection>
-  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" keepAlive="1" name="Consulta - 2024-06-11 07-08-40 (2)" description="Conexión a la consulta '2024-06-11 07-08-40 (2)' en el libro." type="5" refreshedVersion="8" background="1" saveData="1">
+  <connection id="2" keepAlive="1" name="Consulta - 2024-06-11 07-08-40 (2)" description="Conexión a la consulta '2024-06-11 07-08-40 (2)' en el libro." type="5" refreshedVersion="8" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=&quot;2024-06-11 07-08-40 (2)&quot;;Extended Properties=&quot;&quot;" command="SELECT * FROM [2024-06-11 07-08-40 (2)]"/>
   </connection>
 </connections>
@@ -8586,7 +8585,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -8626,10 +8625,10 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -8645,7 +8644,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DatosExternos_1" connectionId="2" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="DatosExternos_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="4">
     <queryTableFields count="2">
       <queryTableField id="2" name="sku" tableColumnId="2"/>
@@ -8656,14 +8655,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla_2024_06_11_07_08_40__2" displayName="Tabla_2024_06_11_07_08_40__2" ref="A1:B1426" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:B1426" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B1426">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla_2024_06_11_07_08_40__2" displayName="Tabla_2024_06_11_07_08_40__2" ref="A1:B1426" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:B1426"/>
+  <sortState ref="A2:B1426">
     <sortCondition ref="A1:A1426"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="sku" queryTableFieldId="2" dataDxfId="0"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="nombre" queryTableFieldId="1" dataDxfId="1"/>
+    <tableColumn id="2" uniqueName="2" name="sku" queryTableFieldId="2" dataDxfId="1"/>
+    <tableColumn id="1" uniqueName="1" name="nombre" queryTableFieldId="1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8965,10 +8964,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1426"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A1408" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>

</xml_diff>